<commit_message>
modified test_cmd_log file to pass test cases
</commit_message>
<xml_diff>
--- a/test_resource/codeextractor_T_T.xlsx
+++ b/test_resource/codeextractor_T_T.xlsx
@@ -97,370 +97,370 @@
     <t>test_guardrails.py_test_validate_return</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_call_subprocess_error(self):_x000D__x000D_
-        """Function to test call_subprocess_error method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        try:_x000D__x000D_
-            guardails_obj.call_subprocess("lshrs")_x000D__x000D_
-        except KeyError:_x000D__x000D_
-            pass_x000D__x000D_
+    <t xml:space="preserve">    def test_call_subprocess_error(self):_x000D_
+        """Function to test call_subprocess_error method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        try:_x000D_
+            guardails_obj.call_subprocess("lshrs")_x000D_
+        except KeyError:_x000D_
+            pass_x000D_
         self.assertNotEqual(guardails_obj.call_subprocess("lshrs"), 0)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_call_subprocess_noerror(self):_x000D__x000D_
-        """Function to test call_subprocess_noerror method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        ret_val = guardails_obj.call_subprocess("dir")_x000D__x000D_
-        self.assertEqual(ret_val, 0)_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_check_pass_fail_success(self):_x000D__x000D_
-        """Function to test check_pass_fail_success method"""_x000D__x000D_
-        list_test = [[10, 100, 10, "Guardrail gating, passed mutation"],_x000D__x000D_
-                     [10, 100, 1, "Guardrail gating, failed mutation"],_x000D__x000D_
-                     [10, 0, 10, "Guardrail gating, failed: mutation test did not run"]]_x000D__x000D_
-        for i, _ in enumerate(list_test):_x000D__x000D_
-            self.assertTrue(list_test[i][3] in self.get_check_pass_fail_status(list_test[i][0],_x000D__x000D_
-                                                                               list_test[i][1], list_test[i][2]))_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_check_report_dir(self, mock_path_exists, mock_mkdir):_x000D__x000D_
-        """Function to test check_report_dir method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        mock_path_exists.return_value = True_x000D__x000D_
-        mock_mkdir.return_value = False_x000D__x000D_
-        guardails_obj.check_report_dir()_x000D__x000D_
+    <t xml:space="preserve">    def test_call_subprocess_noerror(self):_x000D_
+        """Function to test call_subprocess_noerror method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        ret_val = guardails_obj.call_subprocess("dir")_x000D_
+        self.assertEqual(ret_val, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_check_pass_fail_success(self):_x000D_
+        """Function to test check_pass_fail_success method"""_x000D_
+        list_test = [[10, 100, 10, "Guardrail gating, passed mutation"],_x000D_
+                     [10, 100, 1, "Guardrail gating, failed mutation"],_x000D_
+                     [10, 0, 10, "Guardrail gating, failed: mutation test did not run"]]_x000D_
+        for i, _ in enumerate(list_test):_x000D_
+            self.assertTrue(list_test[i][3] in self.get_check_pass_fail_status(list_test[i][0],_x000D_
+                                                                               list_test[i][1], list_test[i][2]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_check_report_dir(self, mock_path_exists, mock_mkdir):_x000D_
+        """Function to test check_report_dir method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        mock_path_exists.return_value = True_x000D_
+        mock_mkdir.return_value = False_x000D_
+        guardails_obj.check_report_dir()_x000D_
         self.assertTrue(mock_mkdir.called)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_file_exists_exit(self):  # pylint: disable=R0201_x000D__x000D_
-        """Function to test file_exists_exit method"""_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            Guardails.file_exists("abc")_x000D__x000D_
+    <t xml:space="preserve">    def test_file_exists_exit(self):  # pylint: disable=R0201_x000D_
+        """Function to test file_exists_exit method"""_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            Guardails.file_exists("abc")_x000D_
             assert exit_mock.called</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_get_all_func_cnn(self):_x000D__x000D_
-        """Function to test get_all_func_cnn method"""_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "CC.xml")_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.get_index_cnn = Mock()_x000D__x000D_
-        guardails_obj.get_index_cnn.return_value = int(2)_x000D__x000D_
-        expec_data = {_x000D__x000D_
-            'get_file_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D__x000D_
-            '\\functiondefextractor\\core_extractor.py:11': '3',_x000D__x000D_
-            'get_function_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D__x000D_
-            '\\functiondefextractor\\core_extractor.py:28': '7'}_x000D__x000D_
-        root = ETree.parse(file_name).getroot()_x000D__x000D_
-        for functions in root.iter('measure'):_x000D__x000D_
-            if functions.attrib['type'] == "Function":_x000D__x000D_
-                assert expec_data == guardails_obj.get_all_func_cnn(functions)_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "CC_test_Func.xml")_x000D__x000D_
-        root = ETree.parse(file_name).getroot()_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            for functions in root.iter('measure'):_x000D__x000D_
-                if functions.attrib['type'] == "Function":_x000D__x000D_
-                    guardails_obj.get_all_func_cnn(functions)_x000D__x000D_
-            file_name = self.get_file_name("test_resource", "CC_test_func_empty.xml")_x000D__x000D_
-            root = ETree.parse(file_name).getroot()_x000D__x000D_
-            for functions in root.iter('measure'):_x000D__x000D_
-                if functions.attrib['type'] == "Function":_x000D__x000D_
-                    guardails_obj.get_all_func_cnn(functions)_x000D__x000D_
-            assert exit_mock.called_x000D__x000D_
-            line = self.get_log_data(2)_x000D__x000D_
-            self.assertTrue(_x000D__x000D_
-                "Guardrail unable to find the tags item/value/name in the report " in line)_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue(_x000D__x000D_
+    <t xml:space="preserve">    def test_get_all_func_cnn(self):_x000D_
+        """Function to test get_all_func_cnn method"""_x000D_
+        file_name = self.get_file_name("test_resource", "CC.xml")_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.get_index_cnn = Mock()_x000D_
+        guardails_obj.get_index_cnn.return_value = int(2)_x000D_
+        expec_data = {_x000D_
+            'get_file_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D_
+            '\\functiondefextractor\\core_extractor.py:11': '3',_x000D_
+            'get_function_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D_
+            '\\functiondefextractor\\core_extractor.py:28': '7'}_x000D_
+        root = ETree.parse(file_name).getroot()_x000D_
+        for functions in root.iter('measure'):_x000D_
+            if functions.attrib['type'] == "Function":_x000D_
+                assert expec_data == guardails_obj.get_all_func_cnn(functions)_x000D_
+        file_name = self.get_file_name("test_resource", "CC_test_Func.xml")_x000D_
+        root = ETree.parse(file_name).getroot()_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            for functions in root.iter('measure'):_x000D_
+                if functions.attrib['type'] == "Function":_x000D_
+                    guardails_obj.get_all_func_cnn(functions)_x000D_
+            file_name = self.get_file_name("test_resource", "CC_test_func_empty.xml")_x000D_
+            root = ETree.parse(file_name).getroot()_x000D_
+            for functions in root.iter('measure'):_x000D_
+                if functions.attrib['type'] == "Function":_x000D_
+                    guardails_obj.get_all_func_cnn(functions)_x000D_
+            assert exit_mock.called_x000D_
+            line = self.get_log_data(2)_x000D_
+            self.assertTrue(_x000D_
+                "Guardrail unable to find the tags item/value/name in the report " in line)_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue(_x000D_
                 "Guardrail unable to find the tags item/value/name in the report file " in line)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_get_index_cnn(self):_x000D__x000D_
-        """Function to test get_index_cnn method"""_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "CC.xml")_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        root = ETree.parse(file_name).getroot()_x000D__x000D_
-        for functions in root.iter('measure'):_x000D__x000D_
-            if functions.attrib['type'] == "Function":_x000D__x000D_
-                assert guardails_obj.get_index_cnn(functions) == 2_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "CC_test_func_empty.xml")_x000D__x000D_
-        root = ETree.parse(file_name).getroot()_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            for functions in root.iter('measure'):_x000D__x000D_
-                if functions.attrib['type'] == "Function":_x000D__x000D_
-                    guardails_obj.get_index_cnn(functions)_x000D__x000D_
-            assert exit_mock.called_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
+    <t xml:space="preserve">    def test_get_index_cnn(self):_x000D_
+        """Function to test get_index_cnn method"""_x000D_
+        file_name = self.get_file_name("test_resource", "CC.xml")_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        root = ETree.parse(file_name).getroot()_x000D_
+        for functions in root.iter('measure'):_x000D_
+            if functions.attrib['type'] == "Function":_x000D_
+                assert guardails_obj.get_index_cnn(functions) == 2_x000D_
+        file_name = self.get_file_name("test_resource", "CC_test_func_empty.xml")_x000D_
+        root = ETree.parse(file_name).getroot()_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            for functions in root.iter('measure'):_x000D_
+                if functions.attrib['type'] == "Function":_x000D_
+                    guardails_obj.get_index_cnn(functions)_x000D_
+            assert exit_mock.called_x000D_
+            line = self.get_log_data(1)_x000D_
             self.assertTrue("Guardrail unable to find the tag CCN in the report " in line)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_coverage(self):_x000D__x000D_
-        """Function to test guardrail_coverage method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_coverage")_x000D__x000D_
-        print(line_2)_x000D__x000D_
-        self.assertTrue("Guardrail , passed Coverage threshold" in line_1)_x000D__x000D_
-        val = r'mypython -m coverage report --fail-under=85'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_coverage(self):_x000D_
+        """Function to test guardrail_coverage method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_coverage")_x000D_
+        print(line_2)_x000D_
+        self.assertTrue("Guardrail , passed Coverage threshold" in line_1)_x000D_
+        val = r'mypython -m coverage report --fail-under=85'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_coverage_fail(self):_x000D__x000D_
-        """Function to test guardrail_coverage_fail method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_coverage")_x000D__x000D_
-        print(line_2)_x000D__x000D_
-        self.assertTrue("Guardrail , failed Coverage threshold" in line_1)_x000D__x000D_
-        val = r'mypython -m coverage report --fail-under=85'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_coverage_fail(self):_x000D_
+        """Function to test guardrail_coverage_fail method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_coverage")_x000D_
+        print(line_2)_x000D_
+        self.assertTrue("Guardrail , failed Coverage threshold" in line_1)_x000D_
+        val = r'mypython -m coverage report --fail-under=85'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_cyclomatic_complexity(self, mock_subproc_call):_x000D__x000D_
-        """Function to test guardrail_cyclomatic_complexity method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.parse_cyclo_report_xml = Mock()_x000D__x000D_
-        guardails_obj.parse_cyclo_report_xml.return_value = {_x000D__x000D_
-            'get_file_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D__x000D_
-            '\\functiondefextractor\\core_extractor.py:11': '3',_x000D__x000D_
-            'get_function_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D__x000D_
-            '\\functiondefextractor\\core_extractor.py:28': '7'}_x000D__x000D_
-        mock_subproc_call.return_value = False_x000D__x000D_
-        guardails_obj.guardrail_cyclomatic_complexity()_x000D__x000D_
-        self.assertTrue(mock_subproc_call.called)_x000D__x000D_
-        line = self.get_log_data(1)_x000D__x000D_
-        self.assertTrue("Guardrail , passed Cyclomatic complexity" in line)_x000D__x000D_
-        mock_subproc_call.return_value = True_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.guardrail_cyclomatic_complexity()_x000D__x000D_
-            line = self.get_log_data(2)_x000D__x000D_
-            self.assertTrue("Guardrail task, failed Cyclomating complexity generation" in line)_x000D__x000D_
-            assert exit_mock_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_guardrail_deadcode(self):_x000D__x000D_
-        """Function to test guardrail_deadcode method"""_x000D__x000D_
-        import os_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_deadcode")_x000D__x000D_
-        self.assertTrue("Guardrail , passed Dead code detection" in line_1)_x000D__x000D_
-        val = r'mypython -m vulture C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\functiondefextractor ' \_x000D__x000D_
-              r'C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\test  --exclude C:\Projects\PythonRepo' \_x000D__x000D_
-              r'\python_sample\FunctionDefExtractor\test --min-confidence 100 &gt;C:\Projects\PythonRepo' \_x000D__x000D_
-              r'\REPORT\deadcode.txt'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_cyclomatic_complexity(self, mock_subproc_call):_x000D_
+        """Function to test guardrail_cyclomatic_complexity method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.parse_cyclo_report_xml = Mock()_x000D_
+        guardails_obj.parse_cyclo_report_xml.return_value = {_x000D_
+            'get_file_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D_
+            '\\functiondefextractor\\core_extractor.py:11': '3',_x000D_
+            'get_function_names(...) at C:\\Projects\\PythonRepo\\python_sample\\FunctionDefExtractor'_x000D_
+            '\\functiondefextractor\\core_extractor.py:28': '7'}_x000D_
+        mock_subproc_call.return_value = False_x000D_
+        guardails_obj.guardrail_cyclomatic_complexity()_x000D_
+        self.assertTrue(mock_subproc_call.called)_x000D_
+        line = self.get_log_data(1)_x000D_
+        self.assertTrue("Guardrail , passed Cyclomatic complexity" in line)_x000D_
+        mock_subproc_call.return_value = True_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.guardrail_cyclomatic_complexity()_x000D_
+            line = self.get_log_data(2)_x000D_
+            self.assertTrue("Guardrail task, failed Cyclomating complexity generation" in line)_x000D_
+            assert exit_mock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_guardrail_deadcode(self):_x000D_
+        """Function to test guardrail_deadcode method"""_x000D_
+        import os_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_deadcode")_x000D_
+        self.assertTrue("Guardrail , passed Dead code detection" in line_1)_x000D_
+        val = r'mypython -m vulture C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\functiondefextractor ' \_x000D_
+              r'C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\test  --exclude C:\Projects\PythonRepo' \_x000D_
+              r'\python_sample\FunctionDefExtractor\test --min-confidence 100 &gt;C:\Projects\PythonRepo' \_x000D_
+              r'\REPORT\deadcode.txt'_x000D_
         self.assertTrue(val.replace("\\", os.sep) in line_2.replace('\\', os.sep).replace("/", os.sep))</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_deadcode_fail(self):_x000D__x000D_
-        """Function to test guardrail_deadcode_fail method"""_x000D__x000D_
-        import os_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_deadcode")_x000D__x000D_
-        self.assertTrue("Guardrail , failed Dead code detection" in line_1)_x000D__x000D_
-        val = r'mypython -m vulture C:\Projects\PythonRepo\python_sample\FunctionDefExtractor' \_x000D__x000D_
-              r'\functiondefextractor ' \_x000D__x000D_
-              r'C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\test  --exclude' \_x000D__x000D_
-              r' C:\Projects\PythonRepo' \_x000D__x000D_
-              r'\python_sample\FunctionDefExtractor\test --min-confidence 100 &gt;C:\Projects' \_x000D__x000D_
-              r'\PythonRepo\REPORT\deadcode.txt'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_deadcode_fail(self):_x000D_
+        """Function to test guardrail_deadcode_fail method"""_x000D_
+        import os_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_deadcode")_x000D_
+        self.assertTrue("Guardrail , failed Dead code detection" in line_1)_x000D_
+        val = r'mypython -m vulture C:\Projects\PythonRepo\python_sample\FunctionDefExtractor' \_x000D_
+              r'\functiondefextractor ' \_x000D_
+              r'C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\test  --exclude' \_x000D_
+              r' C:\Projects\PythonRepo' \_x000D_
+              r'\python_sample\FunctionDefExtractor\test --min-confidence 100 &gt;C:\Projects' \_x000D_
+              r'\PythonRepo\REPORT\deadcode.txt'_x000D_
         self.assertTrue(val.replace('\\', os.sep) in line_2.replace('\\', os.sep).replace("/", os.sep))</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_jscpd(self):_x000D__x000D_
-        """Function to test guardrail_jscpd method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_jscpd")_x000D__x000D_
-        self.assertTrue("Guardrail task, passed Copy Paste Detection report generation" in line_1)_x000D__x000D_
-        val = r'command for sub process:jscpd --min-tokens 20  --ignore C:\Projects\PythonRepo\python_sample' \_x000D__x000D_
-              r'\FunctionDefExtractor\test  --max-lines 100000 --max-size 100mb --reporters "json,html"' \_x000D__x000D_
-              r' --mode "strict" --format "python, java" -o'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_jscpd(self):_x000D_
+        """Function to test guardrail_jscpd method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_jscpd")_x000D_
+        self.assertTrue("Guardrail task, passed Copy Paste Detection report generation" in line_1)_x000D_
+        val = r'command for sub process:jscpd --min-tokens 20  --ignore C:\Projects\PythonRepo\python_sample' \_x000D_
+              r'\FunctionDefExtractor\test  --max-lines 100000 --max-size 100mb --reporters "json,html"' \_x000D_
+              r' --mode "strict" --format "python, java" -o'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_jscpd_fail(self):_x000D__x000D_
-        """Function to test guardrail_jscpd_fail method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_jscpd")_x000D__x000D_
-        self.assertTrue("Guardrail task, failed Copy Paste Detection report generation" in line_1)_x000D__x000D_
-        val = r'command for sub process:jscpd --min-tokens 20  --ignore C:\Projects\PythonRepo\python_sample' \_x000D__x000D_
-              r'\FunctionDefExtractor\test  --max-lines 100000 --max-size 100mb --reporters "json,html" --mode ' \_x000D__x000D_
-              r'"strict" --format "python, java" -o'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_jscpd_fail(self):_x000D_
+        """Function to test guardrail_jscpd_fail method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_jscpd")_x000D_
+        self.assertTrue("Guardrail task, failed Copy Paste Detection report generation" in line_1)_x000D_
+        val = r'command for sub process:jscpd --min-tokens 20  --ignore C:\Projects\PythonRepo\python_sample' \_x000D_
+              r'\FunctionDefExtractor\test  --max-lines 100000 --max-size 100mb --reporters "json,html" --mode ' \_x000D_
+              r'"strict" --format "python, java" -o'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_lint(self, mock_subproc_call):_x000D__x000D_
-        """Function to test guardrail_lint method"""_x000D__x000D_
-        import os_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        global_obj = GuardrailGlobals()_x000D__x000D_
-        mock_subproc_call.return_value = False_x000D__x000D_
-        guardails_obj.lint_ignore = self.get_file_name("test_resource", "pylint_ignore.txt")_x000D__x000D_
-        guardails_obj.generate_files_lint = MagicMock(return_value=" ")_x000D__x000D_
-        global_obj.report_folder = os.getcwd()_x000D__x000D_
-        guardails_obj.guardrail_lint()_x000D__x000D_
-        self.assertTrue(mock_subproc_call.called)_x000D__x000D_
-        line = self.get_log_data(1)_x000D__x000D_
-        self.assertTrue("Guardrail , passed Linting." in str(line))_x000D__x000D_
-        mock_subproc_call.return_value = True_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.guardrail_lint()_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue("Guardrail , failed Linting." in str(line))_x000D__x000D_
-            assert exit_mock_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_lint(self, mock_subproc_call):_x000D_
+        """Function to test guardrail_lint method"""_x000D_
+        import os_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        global_obj = GuardrailGlobals()_x000D_
+        mock_subproc_call.return_value = False_x000D_
+        guardails_obj.lint_ignore = self.get_file_name("test_resource", "pylint_ignore.txt")_x000D_
+        guardails_obj.generate_files_lint = MagicMock(return_value=" ")_x000D_
+        global_obj.report_folder = os.getcwd()_x000D_
+        guardails_obj.guardrail_lint()_x000D_
+        self.assertTrue(mock_subproc_call.called)_x000D_
+        line = self.get_log_data(1)_x000D_
+        self.assertTrue("Guardrail , passed Linting." in str(line))_x000D_
+        mock_subproc_call.return_value = True_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.guardrail_lint()_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue("Guardrail , failed Linting." in str(line))_x000D_
+            assert exit_mock_x000D_
         self.assertTrue(mock_subproc_call.called)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_mutation(self, mock_subproc_call):_x000D__x000D_
-        """Function to test guardrail_mutation method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.parse_mutmut_report_xml = Mock()_x000D__x000D_
-        guardails_obj.parse_mutmut_report_xml.return_value = None_x000D__x000D_
-        mock_subproc_call.return_value = False_x000D__x000D_
-        guardails_obj.guardrail_mutation()_x000D__x000D_
-        self.assertTrue(mock_subproc_call.called)_x000D__x000D_
-        line = self.get_log_data(1)_x000D__x000D_
-        self.assertTrue("Guardrail task, passed Mutation testing report generation." in line)_x000D__x000D_
-        mock_subproc_call.return_value = True_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.guardrail_mutation()_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue("Guardrail task, failed Mutation testing " in line)_x000D__x000D_
-            assert exit_mock_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_guardrail_test(self):_x000D__x000D_
-        """Function to test guardrail_test method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_test")_x000D__x000D_
-        self.assertTrue("Guardrail task, passed Test execution and coverage generation" in line_1)_x000D__x000D_
-        val = r'mypython -m pytest C:\Projects\PythonRepo\python_sample\FunctionDefExtractor' \_x000D__x000D_
-              r' --cov-config=C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\.coveragerc ' \_x000D__x000D_
-              r'--cov-report "html" --cov=C:\Projects\PythonRepo\python_sample' \_x000D__x000D_
-              r'\FunctionDefExtractor\functiondefextractor'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_mutation(self, mock_subproc_call):_x000D_
+        """Function to test guardrail_mutation method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.parse_mutmut_report_xml = Mock()_x000D_
+        guardails_obj.parse_mutmut_report_xml.return_value = None_x000D_
+        mock_subproc_call.return_value = False_x000D_
+        guardails_obj.guardrail_mutation()_x000D_
+        self.assertTrue(mock_subproc_call.called)_x000D_
+        line = self.get_log_data(1)_x000D_
+        self.assertTrue("Guardrail task, passed Mutation testing report generation." in line)_x000D_
+        mock_subproc_call.return_value = True_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.guardrail_mutation()_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue("Guardrail task, failed Mutation testing " in line)_x000D_
+            assert exit_mock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_guardrail_test(self):_x000D_
+        """Function to test guardrail_test method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status(gate="guardrail_test")_x000D_
+        self.assertTrue("Guardrail task, passed Test execution and coverage generation" in line_1)_x000D_
+        val = r'mypython -m pytest C:\Projects\PythonRepo\python_sample\FunctionDefExtractor' \_x000D_
+              r' --cov-config=C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\.coveragerc ' \_x000D_
+              r'--cov-report "html" --cov=C:\Projects\PythonRepo\python_sample' \_x000D_
+              r'\FunctionDefExtractor\functiondefextractor'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_guardrail_test_fail(self):_x000D__x000D_
-        """Function to test guardrail_test_fail method"""_x000D__x000D_
-        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_test")_x000D__x000D_
-        self.assertTrue("Guardrail task, failed Test execution and coverage generation" in line_1)_x000D__x000D_
-        val = r'mypython -m pytest C:\Projects\PythonRepo\python_sample\FunctionDefExtractor ' \_x000D__x000D_
-              r'--cov-config=C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\.coveragerc ' \_x000D__x000D_
-              r'--cov-report "html" --cov=C:\Projects\PythonRepo\python_sample' \_x000D__x000D_
-              r'\FunctionDefExtractor\functiondefextractor'_x000D__x000D_
+    <t xml:space="preserve">    def test_guardrail_test_fail(self):_x000D_
+        """Function to test guardrail_test_fail method"""_x000D_
+        line_1, line_2 = self.get_test_guardrail_gate_status_fail(gate="guardrail_test")_x000D_
+        self.assertTrue("Guardrail task, failed Test execution and coverage generation" in line_1)_x000D_
+        val = r'mypython -m pytest C:\Projects\PythonRepo\python_sample\FunctionDefExtractor ' \_x000D_
+              r'--cov-config=C:\Projects\PythonRepo\python_sample\FunctionDefExtractor\.coveragerc ' \_x000D_
+              r'--cov-report "html" --cov=C:\Projects\PythonRepo\python_sample' \_x000D_
+              r'\FunctionDefExtractor\functiondefextractor'_x000D_
         self.assertTrue(str(val) in line_2)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_list_to_str_folders(self):_x000D__x000D_
-        """Function to test list_to_str_folders method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        self.stub_globals(guardails_obj)_x000D__x000D_
+    <t xml:space="preserve">    def test_list_to_str_folders(self):_x000D_
+        """Function to test list_to_str_folders method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        self.stub_globals(guardails_obj)_x000D_
         self.assertEqual(guardails_obj.list_to_str_folders(), "abc test")</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_mov_cov_report(self, mock_subproc_call, mock_shut_rmtr, mock_shut_mov):_x000D__x000D_
-        """Function to test mov_cov_report method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        process_sub_mock = mock.Mock()_x000D__x000D_
-        patcher_exist = mock.patch('os.path.exists')_x000D__x000D_
-        mock_thing = patcher_exist.start()_x000D__x000D_
-        mock_thing.return_value = True_x000D__x000D_
-        patcher_isdir = mock.patch('os.path.isdir')_x000D__x000D_
-        mock_thing_isdir = patcher_isdir.start()_x000D__x000D_
-        mock_thing_isdir.return_value = True_x000D__x000D_
-        mock_subproc_call.return_value = process_sub_mock_x000D__x000D_
-        mock_shut_rmtr.return_value = process_sub_mock_x000D__x000D_
-        mock_shut_mov.return_value = process_sub_mock_x000D__x000D_
-        guardails_obj.validate_return = self.stub_validate_return_x000D__x000D_
-        guardails_obj.mov_cov_report()_x000D__x000D_
+    <t xml:space="preserve">    def test_mov_cov_report(self, mock_subproc_call, mock_shut_rmtr, mock_shut_mov):_x000D_
+        """Function to test mov_cov_report method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        process_sub_mock = mock.Mock()_x000D_
+        patcher_exist = mock.patch('os.path.exists')_x000D_
+        mock_thing = patcher_exist.start()_x000D_
+        mock_thing.return_value = True_x000D_
+        patcher_isdir = mock.patch('os.path.isdir')_x000D_
+        mock_thing_isdir = patcher_isdir.start()_x000D_
+        mock_thing_isdir.return_value = True_x000D_
+        mock_subproc_call.return_value = process_sub_mock_x000D_
+        mock_shut_rmtr.return_value = process_sub_mock_x000D_
+        mock_shut_mov.return_value = process_sub_mock_x000D_
+        guardails_obj.validate_return = self.stub_validate_return_x000D_
+        guardails_obj.mov_cov_report()_x000D_
         self.assertTrue(mock_subproc_call.called)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_orchestrate_guardrails(self):_x000D__x000D_
-        """Function to test orchestrate_guardrails method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.check_report_dir = Mock()_x000D__x000D_
-        guardails_obj.mov_cov_report = Mock()_x000D__x000D_
-        guardails_obj.mov_cov_report.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.mov_cov_report.return_value)_x000D__x000D_
-        guardails_obj.guardrail_lint = Mock()_x000D__x000D_
-        guardails_obj.guardrail_lint.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_lint.return_value)_x000D__x000D_
-        guardails_obj.guardrail_jscpd = Mock()_x000D__x000D_
-        guardails_obj.guardrail_jscpd.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_jscpd.return_value)_x000D__x000D_
-        guardails_obj.guardrail_test = Mock()_x000D__x000D_
-        guardails_obj.guardrail_test.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_test.return_value)_x000D__x000D_
-        guardails_obj.guardrail_coverage = Mock()_x000D__x000D_
-        guardails_obj.guardrail_coverage.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_coverage.return_value)_x000D__x000D_
-        guardails_obj.guardrail_mutation = Mock()_x000D__x000D_
-        guardails_obj.guardrail_mutation.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_mutation.return_value)_x000D__x000D_
-        guardails_obj.guardrail_deadcode = Mock()_x000D__x000D_
-        guardails_obj.guardrail_deadcode.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_deadcode.return_value)_x000D__x000D_
-        guardails_obj.guardrail_cyclomatic_complexity = Mock()_x000D__x000D_
-        guardails_obj.guardrail_cyclomatic_complexity.return_value = True_x000D__x000D_
-        self.assertTrue(guardails_obj.guardrail_cyclomatic_complexity.return_value)_x000D__x000D_
-        guardails_obj.orchestrate_guardrails()_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_parse_cyclo_report_xml(self):_x000D__x000D_
-        """Function to test parse_cyclo_report_xml method"""_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "CC.xml")_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.get_all_func_cnn = Mock()_x000D__x000D_
-        guardails_obj.get_all_func_cnn.return_value = self.stub_get_all_func_cnn_x000D__x000D_
-        assert guardails_obj.parse_cyclo_report_xml(file_name)_x000D__x000D_
-        file_name = self.get_file_name("test_resourc", "CC.xml")_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.parse_cyclo_report_xml(file_name)_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue("cc.xml report file path" in line)_x000D__x000D_
-            file_name = self.get_file_name("test_resource", "CC_test.xml")_x000D__x000D_
-            guardails_obj.parse_cyclo_report_xml(file_name)_x000D__x000D_
-            file_name = self.get_file_name("test_resource", "CC_test_None.xml")_x000D__x000D_
-            guardails_obj.parse_cyclo_report_xml(file_name)_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue("tags required are not found in cc.xml report file path" in line)_x000D__x000D_
+    <t xml:space="preserve">    def test_orchestrate_guardrails(self):_x000D_
+        """Function to test orchestrate_guardrails method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.check_report_dir = Mock()_x000D_
+        guardails_obj.mov_cov_report = Mock()_x000D_
+        guardails_obj.mov_cov_report.return_value = True_x000D_
+        self.assertTrue(guardails_obj.mov_cov_report.return_value)_x000D_
+        guardails_obj.guardrail_lint = Mock()_x000D_
+        guardails_obj.guardrail_lint.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_lint.return_value)_x000D_
+        guardails_obj.guardrail_jscpd = Mock()_x000D_
+        guardails_obj.guardrail_jscpd.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_jscpd.return_value)_x000D_
+        guardails_obj.guardrail_test = Mock()_x000D_
+        guardails_obj.guardrail_test.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_test.return_value)_x000D_
+        guardails_obj.guardrail_coverage = Mock()_x000D_
+        guardails_obj.guardrail_coverage.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_coverage.return_value)_x000D_
+        guardails_obj.guardrail_mutation = Mock()_x000D_
+        guardails_obj.guardrail_mutation.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_mutation.return_value)_x000D_
+        guardails_obj.guardrail_deadcode = Mock()_x000D_
+        guardails_obj.guardrail_deadcode.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_deadcode.return_value)_x000D_
+        guardails_obj.guardrail_cyclomatic_complexity = Mock()_x000D_
+        guardails_obj.guardrail_cyclomatic_complexity.return_value = True_x000D_
+        self.assertTrue(guardails_obj.guardrail_cyclomatic_complexity.return_value)_x000D_
+        guardails_obj.orchestrate_guardrails()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_parse_cyclo_report_xml(self):_x000D_
+        """Function to test parse_cyclo_report_xml method"""_x000D_
+        file_name = self.get_file_name("test_resource", "CC.xml")_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.get_all_func_cnn = Mock()_x000D_
+        guardails_obj.get_all_func_cnn.return_value = self.stub_get_all_func_cnn_x000D_
+        assert guardails_obj.parse_cyclo_report_xml(file_name)_x000D_
+        file_name = self.get_file_name("test_resourc", "CC.xml")_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.parse_cyclo_report_xml(file_name)_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue("cc.xml report file path" in line)_x000D_
+            file_name = self.get_file_name("test_resource", "CC_test.xml")_x000D_
+            guardails_obj.parse_cyclo_report_xml(file_name)_x000D_
+            file_name = self.get_file_name("test_resource", "CC_test_None.xml")_x000D_
+            guardails_obj.parse_cyclo_report_xml(file_name)_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue("tags required are not found in cc.xml report file path" in line)_x000D_
             assert exit_mock.called</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_parse_jscpd_report_json(self):_x000D__x000D_
-        """Function to test parse_jscpd_report_json method"""_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "jscpd-report.json")_x000D__x000D_
-        guardails_obj.parse_jscpd_report_json(5, file_name)_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D__x000D_
-            file_name = self.get_file_name("test_resource", "jscpd-report_test.json")_x000D__x000D_
-            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D__x000D_
-            file_name = self.get_file_name("test_resource", "jscpd-report_test _error.json")_x000D__x000D_
-            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D__x000D_
-            assert exit_mock.called_x000D__x000D_
-            line = self.get_log_data(3)_x000D__x000D_
-            self.assertTrue("Guardrail gating, failed jscpd." in line)_x000D__x000D_
-            line = self.get_log_data(4)_x000D__x000D_
-            self.assertTrue("Guardrail gating passed jscpd" in line)_x000D__x000D_
-            line = self.get_log_data(2)_x000D__x000D_
-            self.assertTrue("jscpd report not correctly generated" in line)_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
+    <t xml:space="preserve">    def test_parse_jscpd_report_json(self):_x000D_
+        """Function to test parse_jscpd_report_json method"""_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        file_name = self.get_file_name("test_resource", "jscpd-report.json")_x000D_
+        guardails_obj.parse_jscpd_report_json(5, file_name)_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D_
+            file_name = self.get_file_name("test_resource", "jscpd-report_test.json")_x000D_
+            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D_
+            file_name = self.get_file_name("test_resource", "jscpd-report_test _error.json")_x000D_
+            guardails_obj.parse_jscpd_report_json(0, file_name)_x000D_
+            assert exit_mock.called_x000D_
+            line = self.get_log_data(3)_x000D_
+            self.assertTrue("Guardrail gating, failed jscpd." in line)_x000D_
+            line = self.get_log_data(4)_x000D_
+            self.assertTrue("Guardrail gating passed jscpd" in line)_x000D_
+            line = self.get_log_data(2)_x000D_
+            self.assertTrue("jscpd report not correctly generated" in line)_x000D_
+            line = self.get_log_data(1)_x000D_
             self.assertTrue("jscpd report not generated" in line)</t>
   </si>
   <si>
-    <t xml:space="preserve">    def test_parse_mutmut_report_xml(self):_x000D__x000D_
-        """Function to test parse_mutmut_report_xml method"""_x000D__x000D_
-        file_name = self.get_file_name("test_resource", "mutmut.xml")_x000D__x000D_
-        guardails_obj = self.get_guardrails_obj()_x000D__x000D_
-        guardails_obj.parse_mutmut_report_xml(50, file_name)_x000D__x000D_
-        line = self.get_log_data(1)_x000D__x000D_
-        self.assertTrue("Guardrail gating, passed mutation" in str(line))_x000D__x000D_
-        file_name = self.get_file_name("test_resourc", "mutmut.xml")_x000D__x000D_
-        with patch('sys.exit') as exit_mock:_x000D__x000D_
-            guardails_obj.parse_mutmut_report_xml(50, file_name)_x000D__x000D_
-            assert exit_mock.called_x000D__x000D_
-            line = self.get_log_data(1)_x000D__x000D_
-            self.assertTrue("mutmut.xml report file path cound not be found" in line)_x000D_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    def test_validate_return(self):_x000D__x000D_
-        """Function to test validate_return method"""_x000D__x000D_
-        list_test = [[1, "test", True, "Guardrail , failed test."], [0, "test", False, "Guardrail task, passed test."]]_x000D__x000D_
-        for i, _ in enumerate(list_test):_x000D__x000D_
-            assert self.get_validate_return(list_test[i][0], list_test[i][1], list_test[i][2]).strip() \_x000D__x000D_
+    <t xml:space="preserve">    def test_parse_mutmut_report_xml(self):_x000D_
+        """Function to test parse_mutmut_report_xml method"""_x000D_
+        file_name = self.get_file_name("test_resource", "mutmut.xml")_x000D_
+        guardails_obj = self.get_guardrails_obj()_x000D_
+        guardails_obj.parse_mutmut_report_xml(50, file_name)_x000D_
+        line = self.get_log_data(1)_x000D_
+        self.assertTrue("Guardrail gating, passed mutation" in str(line))_x000D_
+        file_name = self.get_file_name("test_resourc", "mutmut.xml")_x000D_
+        with patch('sys.exit') as exit_mock:_x000D_
+            guardails_obj.parse_mutmut_report_xml(50, file_name)_x000D_
+            assert exit_mock.called_x000D_
+            line = self.get_log_data(1)_x000D_
+            self.assertTrue("mutmut.xml report file path cound not be found" in line)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def test_validate_return(self):_x000D_
+        """Function to test validate_return method"""_x000D_
+        list_test = [[1, "test", True, "Guardrail , failed test."], [0, "test", False, "Guardrail task, passed test."]]_x000D_
+        for i, _ in enumerate(list_test):_x000D_
+            assert self.get_validate_return(list_test[i][0], list_test[i][1], list_test[i][2]).strip() \_x000D_
                    == list_test[i][3]</t>
   </si>
 </sst>

</xml_diff>